<commit_message>
Updating Code on FS-014
</commit_message>
<xml_diff>
--- a/cypress/fixtures/upload/bad-address-test.xlsx
+++ b/cypress/fixtures/upload/bad-address-test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\SAFRA.SMCMS.WebUITestAutomation\cypress\fixtures\upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI RYZEN 5\Desktop\V12 MainE2E\SAFRA.SMCMS.WebUITestAutomation\cypress\fixtures\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370FD40E-8845-402A-9A29-D2E8BACF87B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619ECC9F-D734-4990-9E1E-2FE0734423FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Postal Code</t>
   </si>
@@ -42,7 +42,16 @@
     <t>My Mailbox</t>
   </si>
   <si>
-    <t>A30000108</t>
+    <t>200A</t>
+  </si>
+  <si>
+    <t>SGPost</t>
+  </si>
+  <si>
+    <t>102A</t>
+  </si>
+  <si>
+    <t>A300000067</t>
   </si>
 </sst>
 </file>
@@ -78,8 +87,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -98,9 +110,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -138,7 +150,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -244,7 +256,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -386,7 +398,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -397,16 +409,14 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -428,10 +438,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>569933</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>570150</v>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>